<commit_message>
Modification in create tree for data and table totest
</commit_message>
<xml_diff>
--- a/dbs/data/activate/Plantilla_reporte_instructores_V4.xlsx
+++ b/dbs/data/activate/Plantilla_reporte_instructores_V4.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="32">
   <si>
     <t xml:space="preserve">Reporte de Instructores</t>
   </si>
@@ -73,7 +73,7 @@
     <t xml:space="preserve">C.C</t>
   </si>
   <si>
-    <t xml:space="preserve">masutier@gmail.com</t>
+    <t xml:space="preserve">softgarten@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">PRODUCCION DANCISTICA</t>
@@ -88,13 +88,16 @@
     <t xml:space="preserve">Starling Hann</t>
   </si>
   <si>
+    <t xml:space="preserve">info.zanahora@gmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">Frank Alberth</t>
   </si>
   <si>
     <t xml:space="preserve">Moses Red</t>
   </si>
   <si>
-    <t xml:space="preserve">gabrielmasutier@gmail.com</t>
+    <t xml:space="preserve">gmasutier77@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Tatsu</t>
@@ -103,28 +106,16 @@
     <t xml:space="preserve">Yamashiro Katana</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Serif"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Jonathan</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Serif"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Scott</t>
-    </r>
+    <t xml:space="preserve">wernutsnatural@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jonathan Scott</t>
   </si>
   <si>
     <t xml:space="preserve">Crane Scarecrow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">datainquisicion@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -134,7 +125,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -203,10 +194,11 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10.5"/>
+      <u val="single"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="DejaVu Serif"/>
-      <family val="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -214,12 +206,6 @@
       <name val="DejaVu Serif"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10.5"/>
-      <color rgb="FF000000"/>
-      <name val="DejaVu Serif"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -278,7 +264,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -315,23 +301,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -518,21 +492,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:XFD1048576"/>
+  <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="2:25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.08984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="26.47"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="24.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="6.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="26.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="29.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="54.29"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="11" style="1" width="24.09"/>
@@ -619,10 +594,10 @@
       <c r="H4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="9" t="n">
+      <c r="I4" s="7" t="n">
         <v>2500590</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="7" t="s">
         <v>18</v>
       </c>
     </row>
@@ -651,14 +626,14 @@
       <c r="H5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="9" t="n">
+      <c r="I5" s="7" t="n">
         <v>2500598</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" s="1" customFormat="true" ht="15.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
         <v>11</v>
       </c>
@@ -683,14 +658,14 @@
       <c r="H6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="9" t="n">
+      <c r="I6" s="7" t="n">
         <v>2530556</v>
       </c>
       <c r="J6" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="true" ht="15.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -715,14 +690,14 @@
       <c r="H7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="9" t="n">
+      <c r="I7" s="7" t="n">
         <v>2530563</v>
       </c>
       <c r="J7" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" s="1" customFormat="true" ht="15.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
         <v>11</v>
       </c>
@@ -747,14 +722,14 @@
       <c r="H8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="9" t="n">
+      <c r="I8" s="7" t="n">
         <v>2558616</v>
       </c>
       <c r="J8" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" s="1" customFormat="true" ht="15.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
         <v>11</v>
       </c>
@@ -779,14 +754,14 @@
       <c r="H9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="9" t="n">
+      <c r="I9" s="7" t="n">
         <v>2617706</v>
       </c>
       <c r="J9" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" s="1" customFormat="true" ht="15.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" s="1" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
@@ -796,7 +771,7 @@
       <c r="C10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="7" t="s">
         <v>20</v>
       </c>
       <c r="E10" s="7" t="s">
@@ -808,20 +783,17 @@
       <c r="G10" s="7" t="n">
         <v>52123123</v>
       </c>
-      <c r="H10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="9" t="n">
+      <c r="H10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="7" t="n">
         <v>2500598</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="XFB10" s="11"/>
-      <c r="XFC10" s="11"/>
-      <c r="XFD10" s="11"/>
-    </row>
-    <row r="11" s="1" customFormat="true" ht="15.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="11" s="1" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>11</v>
       </c>
@@ -831,7 +803,7 @@
       <c r="C11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="7" t="s">
         <v>20</v>
       </c>
       <c r="E11" s="7" t="s">
@@ -843,20 +815,17 @@
       <c r="G11" s="7" t="n">
         <v>52123123</v>
       </c>
-      <c r="H11" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" s="9" t="n">
+      <c r="H11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="7" t="n">
         <v>2530556</v>
       </c>
       <c r="J11" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="XFB11" s="11"/>
-      <c r="XFC11" s="11"/>
-      <c r="XFD11" s="11"/>
-    </row>
-    <row r="12" s="1" customFormat="true" ht="15.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="12" s="1" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
         <v>11</v>
       </c>
@@ -866,7 +835,7 @@
       <c r="C12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="7" t="s">
         <v>20</v>
       </c>
       <c r="E12" s="7" t="s">
@@ -878,20 +847,17 @@
       <c r="G12" s="7" t="n">
         <v>52123123</v>
       </c>
-      <c r="H12" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="9" t="n">
+      <c r="H12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="7" t="n">
         <v>2617706</v>
       </c>
       <c r="J12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="XFB12" s="11"/>
-      <c r="XFC12" s="11"/>
-      <c r="XFD12" s="11"/>
-    </row>
-    <row r="13" s="1" customFormat="true" ht="15.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="13" s="1" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
         <v>11</v>
       </c>
@@ -901,7 +867,7 @@
       <c r="C13" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="7" t="s">
         <v>20</v>
       </c>
       <c r="E13" s="7" t="s">
@@ -913,20 +879,17 @@
       <c r="G13" s="7" t="n">
         <v>52123123</v>
       </c>
-      <c r="H13" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" s="9" t="n">
+      <c r="H13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="7" t="n">
         <v>2617739</v>
       </c>
       <c r="J13" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="XFB13" s="11"/>
-      <c r="XFC13" s="11"/>
-      <c r="XFD13" s="11"/>
-    </row>
-    <row r="14" s="1" customFormat="true" ht="15.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="14" s="1" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
         <v>11</v>
       </c>
@@ -937,10 +900,10 @@
         <v>13</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>16</v>
@@ -948,31 +911,31 @@
       <c r="G14" s="7" t="n">
         <v>80789789</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I14" s="7" t="n">
+        <v>2500590</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" s="1" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="I14" s="9" t="n">
-        <v>2500590</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" s="1" customFormat="true" ht="15.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>23</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>16</v>
@@ -980,31 +943,31 @@
       <c r="G15" s="7" t="n">
         <v>80789789</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H15" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="7" t="n">
+        <v>2530556</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" s="1" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="I15" s="9" t="n">
-        <v>2530556</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" s="1" customFormat="true" ht="15.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>23</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>16</v>
@@ -1012,31 +975,31 @@
       <c r="G16" s="7" t="n">
         <v>80789789</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="H16" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" s="7" t="n">
+        <v>2558616</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" s="1" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="I16" s="9" t="n">
-        <v>2558616</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" s="1" customFormat="true" ht="15.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>23</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>16</v>
@@ -1044,17 +1007,17 @@
       <c r="G17" s="7" t="n">
         <v>80789789</v>
       </c>
-      <c r="H17" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="I17" s="9" t="n">
+      <c r="H17" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I17" s="7" t="n">
         <v>2617706</v>
       </c>
       <c r="J17" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" s="1" customFormat="true" ht="15.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" s="1" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="s">
         <v>11</v>
       </c>
@@ -1064,11 +1027,11 @@
       <c r="C18" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" s="12" t="s">
+      <c r="D18" s="10" t="s">
         <v>26</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>16</v>
@@ -1076,17 +1039,17 @@
       <c r="G18" s="7" t="n">
         <v>53147147</v>
       </c>
-      <c r="H18" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="I18" s="9" t="n">
+      <c r="H18" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" s="7" t="n">
         <v>2500590</v>
       </c>
       <c r="J18" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" s="1" customFormat="true" ht="15.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" s="1" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
         <v>11</v>
       </c>
@@ -1096,11 +1059,11 @@
       <c r="C19" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" s="12" t="s">
+      <c r="D19" s="10" t="s">
         <v>26</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>16</v>
@@ -1108,17 +1071,17 @@
       <c r="G19" s="7" t="n">
         <v>53147147</v>
       </c>
-      <c r="H19" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="I19" s="9" t="n">
+      <c r="H19" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I19" s="7" t="n">
         <v>2500598</v>
       </c>
       <c r="J19" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" s="1" customFormat="true" ht="15.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" s="1" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
         <v>11</v>
       </c>
@@ -1128,11 +1091,11 @@
       <c r="C20" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="12" t="s">
+      <c r="D20" s="10" t="s">
         <v>26</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>16</v>
@@ -1140,17 +1103,17 @@
       <c r="G20" s="7" t="n">
         <v>53147147</v>
       </c>
-      <c r="H20" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="I20" s="9" t="n">
+      <c r="H20" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" s="7" t="n">
         <v>2530563</v>
       </c>
       <c r="J20" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" s="1" customFormat="true" ht="15.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" s="1" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
         <v>11</v>
       </c>
@@ -1160,11 +1123,11 @@
       <c r="C21" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="12" t="s">
+      <c r="D21" s="10" t="s">
         <v>26</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>16</v>
@@ -1172,17 +1135,17 @@
       <c r="G21" s="7" t="n">
         <v>53147147</v>
       </c>
-      <c r="H21" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="I21" s="9" t="n">
+      <c r="H21" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I21" s="7" t="n">
         <v>2558616</v>
       </c>
       <c r="J21" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" s="1" customFormat="true" ht="15.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" s="1" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
         <v>11</v>
       </c>
@@ -1192,11 +1155,11 @@
       <c r="C22" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="E22" s="12" t="s">
+      <c r="D22" s="10" t="s">
         <v>26</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>16</v>
@@ -1204,17 +1167,17 @@
       <c r="G22" s="7" t="n">
         <v>53147147</v>
       </c>
-      <c r="H22" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="I22" s="9" t="n">
+      <c r="H22" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="7" t="n">
         <v>2617706</v>
       </c>
       <c r="J22" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" s="1" customFormat="true" ht="15.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" s="1" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="7" t="s">
         <v>11</v>
       </c>
@@ -1224,11 +1187,11 @@
       <c r="C23" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="E23" s="12" t="s">
+      <c r="D23" s="10" t="s">
         <v>26</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>16</v>
@@ -1236,17 +1199,17 @@
       <c r="G23" s="7" t="n">
         <v>53147147</v>
       </c>
-      <c r="H23" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="I23" s="9" t="n">
+      <c r="H23" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I23" s="7" t="n">
         <v>2617739</v>
       </c>
       <c r="J23" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" s="1" customFormat="true" ht="15.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" s="1" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="7" t="s">
         <v>11</v>
       </c>
@@ -1256,11 +1219,11 @@
       <c r="C24" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="13" t="s">
-        <v>27</v>
+      <c r="D24" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>16</v>
@@ -1268,17 +1231,17 @@
       <c r="G24" s="7" t="n">
         <v>80369369</v>
       </c>
-      <c r="H24" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I24" s="9" t="n">
+      <c r="H24" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I24" s="7" t="n">
         <v>2500590</v>
       </c>
       <c r="J24" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" s="1" customFormat="true" ht="15.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" s="1" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="s">
         <v>11</v>
       </c>
@@ -1288,11 +1251,11 @@
       <c r="C25" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="13" t="s">
-        <v>27</v>
+      <c r="D25" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>16</v>
@@ -1300,10 +1263,10 @@
       <c r="G25" s="7" t="n">
         <v>80369369</v>
       </c>
-      <c r="H25" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I25" s="9" t="n">
+      <c r="H25" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I25" s="7" t="n">
         <v>2530556</v>
       </c>
       <c r="J25" s="7" t="s">
@@ -1318,30 +1281,6 @@
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="H4" r:id="rId1" display="masutier@gmail.com"/>
-    <hyperlink ref="H5" r:id="rId2" display="masutier@gmail.com"/>
-    <hyperlink ref="H6" r:id="rId3" display="masutier@gmail.com"/>
-    <hyperlink ref="H7" r:id="rId4" display="masutier@gmail.com"/>
-    <hyperlink ref="H8" r:id="rId5" display="masutier@gmail.com"/>
-    <hyperlink ref="H9" r:id="rId6" display="masutier@gmail.com"/>
-    <hyperlink ref="H10" r:id="rId7" display="masutier@gmail.com"/>
-    <hyperlink ref="H11" r:id="rId8" display="masutier@gmail.com"/>
-    <hyperlink ref="H12" r:id="rId9" display="masutier@gmail.com"/>
-    <hyperlink ref="H13" r:id="rId10" display="masutier@gmail.com"/>
-    <hyperlink ref="H14" r:id="rId11" display="gabrielmasutier@gmail.com"/>
-    <hyperlink ref="H15" r:id="rId12" display="gabrielmasutier@gmail.com"/>
-    <hyperlink ref="H16" r:id="rId13" display="gabrielmasutier@gmail.com"/>
-    <hyperlink ref="H17" r:id="rId14" display="gabrielmasutier@gmail.com"/>
-    <hyperlink ref="H18" r:id="rId15" display="gabrielmasutier@gmail.com"/>
-    <hyperlink ref="H19" r:id="rId16" display="gabrielmasutier@gmail.com"/>
-    <hyperlink ref="H20" r:id="rId17" display="gabrielmasutier@gmail.com"/>
-    <hyperlink ref="H21" r:id="rId18" display="gabrielmasutier@gmail.com"/>
-    <hyperlink ref="H22" r:id="rId19" display="gabrielmasutier@gmail.com"/>
-    <hyperlink ref="H23" r:id="rId20" display="gabrielmasutier@gmail.com"/>
-    <hyperlink ref="H24" r:id="rId21" display="masutier@gmail.com"/>
-    <hyperlink ref="H25" r:id="rId22" display="masutier@gmail.com"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>